<commit_message>
Version 1.01, searching UI for missing data in db added
</commit_message>
<xml_diff>
--- a/data_for_the_script.xlsx
+++ b/data_for_the_script.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGCASA\source\repos\angelcasadodnv\Automatizaci-n-de-los-servicios-de-ajuste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EAEFDC-CFE8-41EC-8BD6-696ADE7C4309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793501F5-4B72-4A8B-AAAF-AE9CBCF2ED20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
-    <sheet name="week_week" sheetId="2" r:id="rId2"/>
+    <sheet name="search" sheetId="4" r:id="rId2"/>
+    <sheet name="week_week" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Inital Date</t>
   </si>
@@ -73,7 +74,19 @@
     <t>Nº weeks</t>
   </si>
   <si>
-    <t>2024-01-01</t>
+    <t>2015-01-01</t>
+  </si>
+  <si>
+    <t>Tabla</t>
+  </si>
+  <si>
+    <t>Interval</t>
+  </si>
+  <si>
+    <t>2015-09-05</t>
+  </si>
+  <si>
+    <t>2015-04-06</t>
   </si>
 </sst>
 </file>
@@ -206,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -224,6 +237,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -510,7 +526,7 @@
   <dimension ref="C3:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E4" sqref="E4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -632,13 +648,16 @@
     <mergeCell ref="I4:M5"/>
     <mergeCell ref="E4:F5"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:F17" xr:uid="{97012E19-F876-4A56-9641-BD4533C29C17}">
+  <dataValidations count="3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14:F17" xr:uid="{97012E19-F876-4A56-9641-BD4533C29C17}">
       <formula1>0</formula1>
       <formula2>60</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:E11 D12:E13" xr:uid="{6FC4E2BD-EA08-4CB8-A09C-1D8A4C570B1E}">
       <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:F13" xr:uid="{D81E27F6-07E2-4E90-B493-39B4D2793135}">
+      <formula1>"1,5,10,15,30,60"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -647,11 +666,78 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B81A83D0-B321-40EE-9AF5-0347089177D8}">
+  <dimension ref="C4:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="21.26953125" customWidth="1"/>
+    <col min="4" max="4" width="17.90625" customWidth="1"/>
+    <col min="5" max="5" width="28.08984375" customWidth="1"/>
+    <col min="6" max="6" width="16.08984375" customWidth="1"/>
+    <col min="7" max="7" width="21.08984375" customWidth="1"/>
+    <col min="8" max="8" width="22.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E4:E5"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:H5" xr:uid="{27F8EA84-2B29-4109-87DD-05B69AE7A278}">
+      <formula1>"aFRR_power,aFRR_Energy,RR,mFRR_Energy"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5" xr:uid="{E66D6C4F-DA2C-44A3-AF13-04B697DB5670}">
+      <formula1>"1,5,10,15,30,60"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7582786F-E1B9-433C-BDB0-94FECABABFB6}">
   <dimension ref="C3:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -677,10 +763,10 @@
     </row>
     <row r="5" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D5">
-        <v>120</v>
+        <v>600</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
@@ -764,9 +850,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:E13" xr:uid="{5A3C5E78-CA14-4EBD-A177-E45D9A46F24E}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:F13" xr:uid="{65641E92-8AEA-4AD9-9DBB-F1D63FCA3395}">
-      <formula1>0</formula1>
-      <formula2>60</formula2>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:F13" xr:uid="{65641E92-8AEA-4AD9-9DBB-F1D63FCA3395}">
+      <formula1>"1,5,10,15,30,60"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Big fix when updating data
</commit_message>
<xml_diff>
--- a/data_for_the_script.xlsx
+++ b/data_for_the_script.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGCASA\source\repos\angelcasadodnv\Automatizaci-n-de-los-servicios-de-ajuste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793501F5-4B72-4A8B-AAAF-AE9CBCF2ED20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C4DCA5-86E8-4D98-8D7F-46411F4251CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11175" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>Column C5 AND D5 have to be as "TEXT" data</t>
   </si>
   <si>
-    <t>2023-07-12</t>
-  </si>
-  <si>
     <t>TABLES</t>
   </si>
   <si>
@@ -68,25 +65,28 @@
     <t>Format: Y-m-d</t>
   </si>
   <si>
-    <t>2023-07-01</t>
-  </si>
-  <si>
     <t>Nº weeks</t>
   </si>
   <si>
-    <t>2015-01-01</t>
-  </si>
-  <si>
     <t>Tabla</t>
   </si>
   <si>
     <t>Interval</t>
   </si>
   <si>
-    <t>2015-09-05</t>
-  </si>
-  <si>
-    <t>2015-04-06</t>
+    <t>2015-05-01</t>
+  </si>
+  <si>
+    <t>2015-05-30</t>
+  </si>
+  <si>
+    <t>2024-08-01</t>
+  </si>
+  <si>
+    <t>2024-08-12</t>
+  </si>
+  <si>
+    <t>2021-07-12</t>
   </si>
 </sst>
 </file>
@@ -526,19 +526,19 @@
   <dimension ref="C3:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:F5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.26953125" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="3:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="3:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="6"/>
       <c r="I4" s="4" t="s">
@@ -557,12 +557,12 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
@@ -572,24 +572,24 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="3:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C10" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -601,43 +601,43 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>15</v>
@@ -667,23 +667,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B81A83D0-B321-40EE-9AF5-0347089177D8}">
-  <dimension ref="C4:H5"/>
+  <dimension ref="C4:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.26953125" customWidth="1"/>
-    <col min="4" max="4" width="17.90625" customWidth="1"/>
-    <col min="5" max="5" width="28.08984375" customWidth="1"/>
-    <col min="6" max="6" width="16.08984375" customWidth="1"/>
-    <col min="7" max="7" width="21.08984375" customWidth="1"/>
-    <col min="8" max="8" width="22.26953125" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -691,29 +691,28 @@
         <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5">
         <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -740,55 +739,55 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.36328125" customWidth="1"/>
-    <col min="4" max="4" width="29.1796875" customWidth="1"/>
-    <col min="5" max="5" width="19.36328125" customWidth="1"/>
-    <col min="6" max="6" width="19.81640625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="3:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D5">
-        <v>600</v>
+        <v>469</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="3:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C10" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -800,9 +799,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -811,27 +810,27 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D13" t="b">
         <v>1</v>
       </c>
@@ -839,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Big fix when updating table mfrr
</commit_message>
<xml_diff>
--- a/data_for_the_script.xlsx
+++ b/data_for_the_script.xlsx
@@ -1,33 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGCASA\source\repos\angelcasadodnv\Automatizaci-n-de-los-servicios-de-ajuste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C4DCA5-86E8-4D98-8D7F-46411F4251CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F023BE3A-5F21-4A6B-BDC1-17052724D2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11175" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="search" sheetId="4" r:id="rId2"/>
     <sheet name="week_week" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>Inital Date</t>
   </si>
@@ -74,19 +85,13 @@
     <t>Interval</t>
   </si>
   <si>
-    <t>2015-05-01</t>
-  </si>
-  <si>
-    <t>2015-05-30</t>
-  </si>
-  <si>
-    <t>2024-08-01</t>
-  </si>
-  <si>
-    <t>2024-08-12</t>
-  </si>
-  <si>
-    <t>2021-07-12</t>
+    <t>2015-01-01</t>
+  </si>
+  <si>
+    <t>2015-01-03</t>
+  </si>
+  <si>
+    <t>2015-09-17</t>
   </si>
 </sst>
 </file>
@@ -526,7 +531,7 @@
   <dimension ref="C3:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,10 +564,10 @@
     </row>
     <row r="5" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
@@ -592,10 +597,10 @@
         <v>6</v>
       </c>
       <c r="D10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>15</v>
@@ -612,7 +617,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.25">
@@ -623,10 +628,10 @@
         <v>0</v>
       </c>
       <c r="E12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.25">
@@ -640,7 +645,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -670,7 +675,7 @@
   <dimension ref="C4:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,14 +710,14 @@
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -736,7 +741,7 @@
   <dimension ref="C3:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,10 +767,10 @@
     </row>
     <row r="5" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>469</v>
+        <v>412</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
@@ -790,10 +795,10 @@
         <v>6</v>
       </c>
       <c r="D10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>15</v>
@@ -804,10 +809,10 @@
         <v>7</v>
       </c>
       <c r="D11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>60</v>
@@ -832,10 +837,10 @@
         <v>10</v>
       </c>
       <c r="D13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>60</v>

</xml_diff>

<commit_message>
Using executemany, code is 20x/30x faster
</commit_message>
<xml_diff>
--- a/data_for_the_script.xlsx
+++ b/data_for_the_script.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGCASA\source\repos\angelcasadodnv\Automatizaci-n-de-los-servicios-de-ajuste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F023BE3A-5F21-4A6B-BDC1-17052724D2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F918BB9B-8693-4CDB-92AF-E6EFA825369A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1305" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Inital Date</t>
   </si>
@@ -85,13 +85,19 @@
     <t>Interval</t>
   </si>
   <si>
+    <t>2015-02-07</t>
+  </si>
+  <si>
+    <t>2015-02-01</t>
+  </si>
+  <si>
     <t>2015-01-01</t>
   </si>
   <si>
-    <t>2015-01-03</t>
-  </si>
-  <si>
-    <t>2015-09-17</t>
+    <t>2015-12-02</t>
+  </si>
+  <si>
+    <t>2024-05-29</t>
   </si>
 </sst>
 </file>
@@ -531,7 +537,7 @@
   <dimension ref="C3:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,10 +570,10 @@
     </row>
     <row r="5" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
@@ -625,7 +631,7 @@
         <v>9</v>
       </c>
       <c r="D12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
@@ -675,7 +681,7 @@
   <dimension ref="C4:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,17 +713,17 @@
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5">
         <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -741,7 +747,7 @@
   <dimension ref="C3:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,10 +773,10 @@
     </row>
     <row r="5" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D5">
-        <v>412</v>
+        <v>5</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
@@ -795,10 +801,10 @@
         <v>6</v>
       </c>
       <c r="D10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>15</v>
@@ -823,10 +829,10 @@
         <v>9</v>
       </c>
       <c r="D12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>60</v>

</xml_diff>